<commit_message>
Verificando email com retorno de erro
</commit_message>
<xml_diff>
--- a/files/PlanilhaNovosFuncionarios.xlsx
+++ b/files/PlanilhaNovosFuncionarios.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7650" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
@@ -59,17 +59,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -416,8 +416,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="28.7109375"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="32.140625"/>
+    <col width="28.7109375" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="32.140625" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -458,7 +458,7 @@
       <c r="B3" s="2" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.787401575" footer="0.31496062" header="0.31496062" left="0.511811024" right="0.511811024" top="0.787401575"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Variaveis de Ambiente/ Criptografia da senha/ Dicionário ISO 8859-1/ Arquivo bat
</commit_message>
<xml_diff>
--- a/files/PlanilhaNovosFuncionarios.xlsx
+++ b/files/PlanilhaNovosFuncionarios.xlsx
@@ -421,7 +421,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -451,29 +451,29 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>D=F3ris Andressa Moura Luvizute</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>doriluvizute@gmail.com</t>
+          <t>Bruno  da Silva</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>dorisluvizute@gmail.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Email inválido</t>
+          <t>ENVIADO</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Bruno  da Silva</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>dorisluvizute@gmail.com</t>
+          <t>Matheus Diniz</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>matheusinhodinizinho@gmail.com</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -485,17 +485,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Matheus Diniz</t>
+          <t>Dóris Andressa Moura Luvizute</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>matheusinhodinizinho@gmail.com</t>
+          <t>doriluvizute@gmail.com</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ENVIADO</t>
+          <t>Email inválido</t>
         </is>
       </c>
     </row>

</xml_diff>